<commit_message>
Added test case 2
</commit_message>
<xml_diff>
--- a/test cases/test_case_1.xlsx
+++ b/test cases/test_case_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\20141\OneDrive\Bureaublad\MSc_1\Operations Optimisation\Assignment\AE4441-16_Assignment\test cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AE9915F-A907-41E7-B0A8-DB4B71D88CAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D92C1C7-A13E-40AF-95E7-A3E17A7DE331}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Node Connections" sheetId="1" r:id="rId1"/>
@@ -376,8 +376,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -479,7 +479,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -563,8 +563,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D5149B8-330A-4152-9750-499E63406303}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O13" sqref="O13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>